<commit_message>
upd prst and zapis
</commit_message>
<xml_diff>
--- a/черновик/Ekonomicheskiy_raschet_po_vyyavlennym_klyuchevym_kharakteristikam (1).xlsx
+++ b/черновик/Ekonomicheskiy_raschet_po_vyyavlennym_klyuchevym_kharakteristikam (1).xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\промтех\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sever.ok\Documents\GitHub\sjc2021_promtech\черновик\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4244C6FE-9C38-49BE-8353-F67A474CDF85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="сравнение" sheetId="1" r:id="rId1"/>
     <sheet name="время и т.д." sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -66,12 +67,6 @@
     <t>Модуль служебных систем</t>
   </si>
   <si>
-    <t>Солнечные батареи</t>
-  </si>
-  <si>
-    <t>Доска Magnetorquer iMTQ</t>
-  </si>
-  <si>
     <t>УКВ-восходящий/УВЧ-нисходящий полнодуплексный трансивер</t>
   </si>
   <si>
@@ -81,9 +76,6 @@
     <t>от 293480 до 558206</t>
   </si>
   <si>
-    <t>ISIS на бортовом компьютере</t>
-  </si>
-  <si>
     <t>от 391307 до 609194</t>
   </si>
   <si>
@@ -93,9 +85,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Стоимость полосы пропускания на Мгц в месяц</t>
-  </si>
-  <si>
     <t>Стоимость транспартировки</t>
   </si>
   <si>
@@ -166,13 +155,25 @@
   </si>
   <si>
     <t>Затраты на создание копрпуса (5кг)</t>
+  </si>
+  <si>
+    <t>Солнечная панель (торцевая)</t>
+  </si>
+  <si>
+    <t>Солнечная батарея (боковая)</t>
+  </si>
+  <si>
+    <t>Плата магнитной стабилизации</t>
+  </si>
+  <si>
+    <t>On-Board Computer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -234,8 +235,15 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,8 +274,14 @@
         <bgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -364,11 +378,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -436,6 +465,31 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -456,7 +510,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -469,31 +522,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -708,28 +757,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.4">
+    <row r="1" spans="1:12" ht="25.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -742,7 +791,7 @@
       <c r="F1" s="4"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="39.6">
+    <row r="2" spans="1:12" ht="38.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -761,12 +810,12 @@
       <c r="H2" s="6"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:12" ht="13.2">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:12" ht="12.75">
+      <c r="A3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>45</v>
+      <c r="B3" s="39" t="s">
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -780,8 +829,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="39" customHeight="1">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
@@ -789,307 +838,308 @@
         <v>10</v>
       </c>
       <c r="E4" s="2">
-        <v>1635</v>
+        <v>33000</v>
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:12" ht="26.4">
-      <c r="A5" s="29"/>
-      <c r="B5" s="31" t="s">
+    <row r="5" spans="1:12" ht="39" customHeight="1">
+      <c r="A5" s="40"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="2"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" ht="25.5">
+      <c r="A6" s="40"/>
+      <c r="B6" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="2">
+        <v>177867</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="25.5">
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1">
+        <v>711467</v>
+      </c>
+      <c r="E7" s="1">
+        <v>711467</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="63.75">
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1">
-        <v>177867</v>
-      </c>
-      <c r="E5" s="1">
-        <f>PRODUCT(D5*6)</f>
-        <v>1067202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="26.4">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="1" t="s">
+      <c r="D8" s="1">
+        <v>755934</v>
+      </c>
+      <c r="E8" s="22">
+        <v>755934</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="38.25">
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1">
-        <v>711467</v>
-      </c>
-      <c r="E6" s="1">
-        <v>711467</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="66">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1">
-        <v>755934</v>
-      </c>
-      <c r="E7" s="22">
-        <v>755934</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="39.6">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="11" t="s">
+      <c r="E9" s="22">
+        <v>293480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="25.5">
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E10" s="23">
+        <v>391307</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" ht="12.75">
+      <c r="A11" s="40"/>
+      <c r="B11" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="22">
-        <v>293480</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="26.4">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="36"/>
+      <c r="D11" s="9">
+        <v>753100</v>
+      </c>
+      <c r="E11" s="9">
+        <v>753100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="12.75">
+      <c r="A12" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="9">
+        <v>25000</v>
+      </c>
+      <c r="E12" s="12">
+        <f>PRODUCT(D12*3)</f>
+        <v>75000</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="13" spans="1:12" ht="12.75">
+      <c r="A13" s="52"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+    </row>
+    <row r="14" spans="1:12" ht="12.75">
+      <c r="A14" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="23">
-        <v>391307</v>
-      </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" ht="13.2">
-      <c r="A10" s="29"/>
-      <c r="B10" s="24" t="s">
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="51">
+        <v>374000</v>
+      </c>
+      <c r="E14" s="51">
+        <v>374000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="25.5">
+      <c r="A15" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="9">
-        <v>753100</v>
-      </c>
-      <c r="E10" s="9">
-        <v>753100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="13.2">
-      <c r="A11" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="9">
-        <v>25000</v>
-      </c>
-      <c r="E11" s="12">
-        <f>PRODUCT(D11*3)</f>
-        <v>75000</v>
-      </c>
-      <c r="G11" s="13" t="s">
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="13.2">
-      <c r="A12" s="33" t="s">
+      <c r="E15" s="1">
+        <v>744300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="12.75">
+      <c r="A16" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="9">
-        <v>260530</v>
-      </c>
-      <c r="E12" s="9">
-        <v>260530</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="13.2">
-      <c r="A13" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="9">
-        <v>374000</v>
-      </c>
-      <c r="E13" s="9">
-        <v>374000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="26.4">
-      <c r="A14" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="1">
-        <v>744300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="13.2">
-      <c r="A15" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="14">
-        <f>SUM(E3:E14)</f>
-        <v>5429555</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="13.2">
-      <c r="C16" s="11"/>
-    </row>
-    <row r="17" spans="3:10" ht="13.2">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="14">
+        <f>SUM(E3:E15)</f>
+        <v>4133188</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" ht="12.75">
       <c r="C17" s="11"/>
     </row>
-    <row r="18" spans="3:10" ht="13.2">
+    <row r="18" spans="3:10" ht="12.75">
       <c r="C18" s="11"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-    </row>
-    <row r="19" spans="3:10" ht="13.2">
+    </row>
+    <row r="19" spans="3:10" ht="12.75">
       <c r="C19" s="11"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="41"/>
-    </row>
-    <row r="20" spans="3:10" ht="13.2">
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="3:10" ht="12.75">
       <c r="C20" s="11"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-    </row>
-    <row r="21" spans="3:10" ht="13.2">
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-    </row>
-    <row r="22" spans="3:10" ht="13.2">
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-    </row>
-    <row r="23" spans="3:10" ht="13.2">
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-    </row>
-    <row r="24" spans="3:10" ht="13.2">
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-    </row>
-    <row r="25" spans="3:10" ht="13.2">
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-    </row>
-    <row r="26" spans="3:10" ht="13.8">
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="44"/>
-    </row>
-    <row r="27" spans="3:10" ht="13.2">
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-    </row>
-    <row r="28" spans="3:10" ht="13.2">
-      <c r="F28" s="40"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
-    </row>
-    <row r="29" spans="3:10" ht="13.2">
-      <c r="F29" s="47"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-    </row>
-    <row r="30" spans="3:10" ht="13.2">
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-    </row>
-    <row r="31" spans="3:10" ht="13.2">
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-    </row>
-    <row r="32" spans="3:10" ht="13.2">
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-    </row>
-    <row r="33" spans="6:10" ht="13.2">
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="44"/>
-    </row>
-    <row r="34" spans="6:10" ht="13.2">
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="44"/>
-    </row>
-    <row r="35" spans="6:10" ht="15.75" customHeight="1">
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="3:10" ht="12.75">
+      <c r="C21" s="11"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+    </row>
+    <row r="22" spans="3:10" ht="12.75">
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="3:10" ht="12.75">
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+    </row>
+    <row r="24" spans="3:10" ht="12.75">
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+    </row>
+    <row r="25" spans="3:10" ht="12.75">
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+    </row>
+    <row r="26" spans="3:10" ht="12.75">
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+    </row>
+    <row r="27" spans="3:10" ht="14.25">
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+    </row>
+    <row r="28" spans="3:10" ht="12.75">
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+    </row>
+    <row r="29" spans="3:10" ht="12.75">
+      <c r="F29" s="26"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+    </row>
+    <row r="30" spans="3:10" ht="12.75">
+      <c r="F30" s="33"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+    </row>
+    <row r="31" spans="3:10" ht="12.75">
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+    </row>
+    <row r="32" spans="3:10" ht="12.75">
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+    </row>
+    <row r="33" spans="6:10" ht="12.75">
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+    </row>
+    <row r="34" spans="6:10" ht="12.75">
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="30"/>
+    </row>
+    <row r="35" spans="6:10" ht="12.75">
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+    </row>
+    <row r="36" spans="6:10" ht="15.75" customHeight="1">
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A3:A11"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1097,59 +1147,59 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="39.6">
+    <row r="1" spans="1:10" ht="38.25">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I1" s="19"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="2" spans="1:10" ht="13.2">
+    <row r="2" spans="1:10" ht="12.75">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2">
         <v>1.5</v>
@@ -1164,22 +1214,22 @@
         <f>PRODUCT(C2:E2)</f>
         <v>16.2</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="39">
         <v>1000</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="39">
         <f>SUM(F2:G3)</f>
         <v>1016.2</v>
       </c>
       <c r="I2" s="19"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:10" ht="13.2">
+    <row r="3" spans="1:10" ht="12.75">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2">
         <v>0.5</v>
@@ -1193,14 +1243,14 @@
       <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="19"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" ht="13.2">
+    <row r="4" spans="1:10" ht="12.75">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -1226,12 +1276,12 @@
       <c r="I4" s="19"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="1:10" ht="39.6">
+    <row r="5" spans="1:10" ht="38.25">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -1256,12 +1306,12 @@
       <c r="I5" s="19"/>
       <c r="J5" s="16"/>
     </row>
-    <row r="6" spans="1:10" ht="13.2">
+    <row r="6" spans="1:10" ht="12.75">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2">
         <v>1.5</v>
@@ -1284,14 +1334,14 @@
       <c r="I6" s="19"/>
       <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="1:10" ht="13.2">
-      <c r="A7" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="37"/>
+    <row r="7" spans="1:10" ht="12.75">
+      <c r="A7" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="21">
         <f>SUM(F2:F6)</f>
         <v>150.59999999999997</v>
@@ -1304,7 +1354,7 @@
       <c r="I7" s="19"/>
       <c r="J7" s="16"/>
     </row>
-    <row r="8" spans="1:10" ht="13.2">
+    <row r="8" spans="1:10" ht="12.75">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -1316,16 +1366,16 @@
       <c r="I8" s="19"/>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="1:10" ht="13.2">
+    <row r="9" spans="1:10" ht="12.75">
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10" ht="13.2">
+    <row r="10" spans="1:10" ht="12.75">
       <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="1:10" ht="13.2">
+    <row r="11" spans="1:10" ht="12.75">
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="1:10" ht="13.2">
+    <row r="12" spans="1:10" ht="12.75">
       <c r="J12" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prst and xlsx upd
</commit_message>
<xml_diff>
--- a/черновик/Ekonomicheskiy_raschet_po_vyyavlennym_klyuchevym_kharakteristikam (1).xlsx
+++ b/черновик/Ekonomicheskiy_raschet_po_vyyavlennym_klyuchevym_kharakteristikam (1).xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sever.ok\Documents\GitHub\sjc2021_promtech\черновик\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniil Sevryuk\Documents\GitHub\sjc2021_promtech\черновик\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4244C6FE-9C38-49BE-8353-F67A474CDF85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F5F886-9B33-4E27-89EA-2301D5459AD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17880" yWindow="5100" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="сравнение" sheetId="1" r:id="rId1"/>
-    <sheet name="время и т.д." sheetId="2" r:id="rId2"/>
+    <sheet name="общая таблица" sheetId="1" r:id="rId1"/>
+    <sheet name="время и электропотребление" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Исскуственный спутник</t>
   </si>
@@ -76,9 +78,6 @@
     <t>от 293480 до 558206</t>
   </si>
   <si>
-    <t>от 391307 до 609194</t>
-  </si>
-  <si>
     <t>Стоимость блоков</t>
   </si>
   <si>
@@ -121,33 +120,18 @@
     <t>Всего руб за вид деятельности</t>
   </si>
   <si>
-    <t>Разогрев металла</t>
-  </si>
-  <si>
     <t xml:space="preserve">Плавильная печь </t>
   </si>
   <si>
-    <t>Литье корпуса</t>
-  </si>
-  <si>
     <t>Форма</t>
   </si>
   <si>
-    <t>Остывание металла</t>
-  </si>
-  <si>
     <t>Фрезеровка</t>
   </si>
   <si>
     <t xml:space="preserve">Фрезер "HAAS - DM-1 4-Axis CNC Milling Machine" </t>
   </si>
   <si>
-    <t>Сбор кубсата</t>
-  </si>
-  <si>
-    <t>Отвертка</t>
-  </si>
-  <si>
     <t>Итого:</t>
   </si>
   <si>
@@ -160,20 +144,26 @@
     <t>Солнечная панель (торцевая)</t>
   </si>
   <si>
-    <t>Солнечная батарея (боковая)</t>
-  </si>
-  <si>
     <t>Плата магнитной стабилизации</t>
   </si>
   <si>
     <t>On-Board Computer</t>
+  </si>
+  <si>
+    <t>от 386100 до 601087</t>
+  </si>
+  <si>
+    <t>Литьё</t>
+  </si>
+  <si>
+    <t>Солнечная панель (боковая)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -242,6 +232,12 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -397,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -491,6 +487,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -507,10 +524,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -522,27 +553,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -761,24 +780,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.5">
+    <row r="1" spans="1:12" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +810,7 @@
       <c r="F1" s="4"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="38.25">
+    <row r="2" spans="1:12" ht="14.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -811,11 +830,11 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:12" ht="12.75">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>41</v>
+      <c r="B3" s="46" t="s">
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -828,9 +847,9 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="39" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
+    <row r="4" spans="1:12" ht="36" customHeight="1">
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
@@ -842,46 +861,54 @@
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:12" ht="39" customHeight="1">
-      <c r="A5" s="40"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="2"/>
+    <row r="5" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A5" s="47"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="12">
+        <v>38000</v>
+      </c>
+      <c r="E5" s="2">
+        <f>SUM(D5*2)</f>
+        <v>76000</v>
+      </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:12" ht="25.5">
-      <c r="A6" s="40"/>
-      <c r="B6" s="42" t="s">
+    <row r="6" spans="1:12" ht="12.75">
+      <c r="A6" s="47"/>
+      <c r="B6" s="49" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2">
-        <v>177867</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" ht="25.5">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="56" t="s">
-        <v>44</v>
+        <v>34100</v>
+      </c>
+      <c r="E6" s="1">
+        <f>SUM(D6*4)</f>
+        <v>136400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="12.75">
+      <c r="A7" s="47"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="35" t="s">
+        <v>37</v>
       </c>
       <c r="D7" s="1">
-        <v>711467</v>
+        <v>702000</v>
       </c>
       <c r="E7" s="1">
-        <v>711467</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="63.75">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="1" t="s">
+        <v>702000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="63.75" customHeight="1">
+      <c r="A8" s="47"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="35" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="1">
@@ -891,10 +918,10 @@
         <v>755934</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="38.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="11" t="s">
+    <row r="9" spans="1:12" ht="38.25" customHeight="1">
+      <c r="A9" s="47"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="41" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -904,27 +931,27 @@
         <v>293480</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="25.5">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
+    <row r="10" spans="1:12" ht="25.5" customHeight="1">
+      <c r="A10" s="47"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>39</v>
       </c>
       <c r="E10" s="23">
-        <v>391307</v>
+        <v>386100</v>
       </c>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" ht="12.75">
-      <c r="A11" s="40"/>
-      <c r="B11" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="36"/>
+      <c r="A11" s="47"/>
+      <c r="B11" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="43"/>
       <c r="D11" s="9">
         <v>753100</v>
       </c>
@@ -933,11 +960,11 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="12.75">
-      <c r="A12" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
+      <c r="A12" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="9">
         <v>25000</v>
       </c>
@@ -946,90 +973,90 @@
         <v>75000</v>
       </c>
       <c r="G12" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="12.75">
+      <c r="A13" s="53" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="12.75">
-      <c r="A13" s="52"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="38">
+        <v>17000</v>
+      </c>
+      <c r="E13" s="38">
+        <v>17000</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="12.75">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="51">
-        <v>374000</v>
-      </c>
-      <c r="E14" s="51">
-        <v>374000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="25.5">
-      <c r="A15" s="35" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="1" t="s">
+      <c r="E14" s="1">
+        <v>744300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="12.75">
+      <c r="A15" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="1">
-        <v>744300</v>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="14">
+        <f>SUM(E3:E14)</f>
+        <v>3973914</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12.75">
-      <c r="A16" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="14">
-        <f>SUM(E3:E15)</f>
-        <v>4133188</v>
-      </c>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" spans="3:10" ht="12.75">
       <c r="C17" s="11"/>
     </row>
     <row r="18" spans="3:10" ht="12.75">
       <c r="C18" s="11"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
     </row>
     <row r="19" spans="3:10" ht="12.75">
       <c r="C19" s="11"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
     </row>
     <row r="20" spans="3:10" ht="12.75">
       <c r="C20" s="11"/>
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="27"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
     </row>
     <row r="21" spans="3:10" ht="12.75">
-      <c r="C21" s="11"/>
       <c r="F21" s="25"/>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
     </row>
     <row r="22" spans="3:10" ht="12.75">
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
       <c r="H22" s="25"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
     </row>
     <row r="23" spans="3:10" ht="12.75">
       <c r="F23" s="25"/>
@@ -1052,38 +1079,38 @@
       <c r="I25" s="30"/>
       <c r="J25" s="30"/>
     </row>
-    <row r="26" spans="3:10" ht="12.75">
+    <row r="26" spans="3:10" ht="14.25">
       <c r="F26" s="25"/>
       <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="30"/>
       <c r="J26" s="30"/>
     </row>
-    <row r="27" spans="3:10" ht="14.25">
+    <row r="27" spans="3:10" ht="12.75">
       <c r="F27" s="25"/>
       <c r="G27" s="25"/>
-      <c r="H27" s="31"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="30"/>
       <c r="J27" s="30"/>
     </row>
     <row r="28" spans="3:10" ht="12.75">
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
       <c r="I28" s="30"/>
       <c r="J28" s="30"/>
     </row>
     <row r="29" spans="3:10" ht="12.75">
-      <c r="F29" s="26"/>
+      <c r="F29" s="33"/>
       <c r="G29" s="32"/>
       <c r="H29" s="32"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
     </row>
     <row r="30" spans="3:10" ht="12.75">
-      <c r="F30" s="33"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
       <c r="I30" s="29"/>
       <c r="J30" s="29"/>
     </row>
@@ -1105,41 +1132,33 @@
       <c r="F33" s="25"/>
       <c r="G33" s="25"/>
       <c r="H33" s="25"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="30"/>
     </row>
     <row r="34" spans="6:10" ht="12.75">
       <c r="F34" s="25"/>
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
-      <c r="I34" s="34"/>
+      <c r="I34" s="30"/>
       <c r="J34" s="30"/>
     </row>
-    <row r="35" spans="6:10" ht="12.75">
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-    </row>
-    <row r="36" spans="6:10" ht="15.75" customHeight="1">
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
+    <row r="35" spans="6:10" ht="15.75" customHeight="1">
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:D16"/>
+  <mergeCells count="8">
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:D15"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1151,10 +1170,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1168,68 +1187,66 @@
   <sheetData>
     <row r="1" spans="1:10" ht="38.25">
       <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="I1" s="19"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:10" ht="12.75">
-      <c r="A2" s="2" t="s">
-        <v>30</v>
+      <c r="A2" s="61" t="s">
+        <v>40</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2">
         <v>1.5</v>
       </c>
       <c r="D2" s="2">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="F2" s="2">
+        <v>5.47</v>
+      </c>
+      <c r="E2" s="40">
+        <v>1300</v>
+      </c>
+      <c r="F2" s="40">
         <f>PRODUCT(C2:E2)</f>
-        <v>16.2</v>
-      </c>
-      <c r="G2" s="39">
-        <v>1000</v>
-      </c>
-      <c r="H2" s="39">
+        <v>10666.5</v>
+      </c>
+      <c r="G2" s="56">
+        <v>1500</v>
+      </c>
+      <c r="H2" s="56">
         <f>SUM(F2:G3)</f>
-        <v>1016.2</v>
+        <v>12166.5</v>
       </c>
       <c r="I2" s="19"/>
       <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:10" ht="12.75">
-      <c r="A3" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="A3" s="62"/>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2">
         <v>0.5</v>
@@ -1243,15 +1260,13 @@
       <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
       <c r="I3" s="19"/>
       <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" ht="12.75">
-      <c r="A4" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="A4" s="63"/>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1278,96 +1293,71 @@
     </row>
     <row r="5" spans="1:10" ht="38.25">
       <c r="A5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>32</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
       </c>
       <c r="D5" s="2">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2">
+        <v>5.47</v>
+      </c>
+      <c r="E5" s="39">
         <v>11.2</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="39">
         <f>PRODUCT(C5:E5)</f>
-        <v>134.39999999999998</v>
-      </c>
-      <c r="G5" s="2">
+        <v>122.52799999999999</v>
+      </c>
+      <c r="G5" s="39">
         <v>1500</v>
       </c>
-      <c r="H5" s="2">
-        <f>SUM(F5:G6)</f>
-        <v>1634.4</v>
+      <c r="H5" s="39">
+        <f>SUM(F5:G5)</f>
+        <v>1622.528</v>
       </c>
       <c r="I5" s="19"/>
       <c r="J5" s="16"/>
     </row>
     <row r="6" spans="1:10" ht="12.75">
-      <c r="A6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>10</v>
+      <c r="A6" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="21">
+        <f>SUM(F2:F5)</f>
+        <v>10789.028</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="18">
+        <f>SUM(H2:H5)</f>
+        <v>13789.028</v>
       </c>
       <c r="I6" s="19"/>
       <c r="J6" s="16"/>
     </row>
     <row r="7" spans="1:10" ht="12.75">
-      <c r="A7" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="21">
-        <f>SUM(F2:F6)</f>
-        <v>150.59999999999997</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="18">
-        <f>SUM(H2:H6)</f>
-        <v>2650.6000000000004</v>
-      </c>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
       <c r="I7" s="19"/>
-      <c r="J7" s="16"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:10" ht="12.75">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="17"/>
+      <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="12.75">
-      <c r="J9" s="16"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:10" ht="12.75">
       <c r="J10" s="17"/>
@@ -1375,14 +1365,12 @@
     <row r="11" spans="1:10" ht="12.75">
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75">
-      <c r="J12" s="17"/>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
-    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A2:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>